<commit_message>
hobbies and programs loaded
</commit_message>
<xml_diff>
--- a/backend_onboarding/API/DataSource/hobbies.xlsx
+++ b/backend_onboarding/API/DataSource/hobbies.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/priscilla_layarda_mail_utoronto_ca/Documents/MeetUT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gordonlin/Documents/meetUT/backend_onboarding/API/DataSource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CA50EFF-6C09-408D-9AC8-09A01E291E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C1DAE8-BD15-EB4D-88C5-59891277028F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="460" windowWidth="22240" windowHeight="17540" xr2:uid="{5DFB22DC-6E34-1B48-A01D-064FA6B0DFC0}"/>
+    <workbookView xWindow="6180" yWindow="500" windowWidth="22240" windowHeight="16340" xr2:uid="{5DFB22DC-6E34-1B48-A01D-064FA6B0DFC0}"/>
   </bookViews>
   <sheets>
     <sheet name="cleaned up" sheetId="2" r:id="rId1"/>
-    <sheet name="raw" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
-  <si>
-    <t>Categories</t>
-  </si>
-  <si>
-    <t>Examples</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>  Fitness</t>
   </si>
@@ -131,70 +124,13 @@
   </si>
   <si>
     <t>Amateur radio, Auto audiophilia, Book restoration, Computer programming, Electronics, Gunsmithing, High-power rocketry, Home building, Knife making, Soapmaking, Vehicle restoration</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Sub-Category</t>
-  </si>
-  <si>
-    <t>Hobbies</t>
-  </si>
-  <si>
-    <t>Collecting</t>
-  </si>
-  <si>
-    <t>  Physical</t>
-  </si>
-  <si>
-    <t>Action figures, Antiquities, Art, Books, Cards, Coins, Comic books, Deltiology (postcards), Elements, Flags, Flowers (pressed), Insects, Mineral, Movie and movie memorabilia, Stamps (Philately), Sea glass, Seashells, Stones, Toys, Video games, Vintage cars</t>
-  </si>
-  <si>
-    <t>  Record</t>
-  </si>
-  <si>
-    <t>Genealogy, Scrapbooking, Movie and movie memorabilia, Music/Audio Records, Video games</t>
-  </si>
-  <si>
-    <t>  Spotting</t>
-  </si>
-  <si>
-    <t>Aircraft spotting, Amateur astronomy, Bird watching, Bus spotting, Dowsing (ground water), Foraging, Geocaching (GPS), Ghost hunting, Gongoozling (canals), Herping (reptiles), Metal detecting, Microscopy, Mushroom hunting/mycology, Satellite watching, Shortwave listening, Train spotting</t>
-  </si>
-  <si>
-    <t>Making</t>
-  </si>
-  <si>
-    <t>Activity</t>
-  </si>
-  <si>
-    <t>  Animal</t>
-  </si>
-  <si>
-    <t>Animal fancy, Beekeeping, Fishing, Fishkeeping, Herp keeping, Horseback riding, Hunting, Pet, Whale watching</t>
-  </si>
-  <si>
-    <t>  Outdoor</t>
-  </si>
-  <si>
-    <t>Play</t>
-  </si>
-  <si>
-    <t>Arts</t>
-  </si>
-  <si>
-    <t>Source:</t>
-  </si>
-  <si>
-    <t>https://hobbycue.com/hobbies/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -539,19 +475,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F321CCB-32CC-2C43-B954-7AC19AEB7E48}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.625" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -567,7 +503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -575,7 +511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -583,7 +519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -591,7 +527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -599,7 +535,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -607,7 +543,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -615,7 +551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -623,7 +559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -631,7 +567,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -639,7 +575,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -647,7 +583,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -655,7 +591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -663,224 +599,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7F0296-0F87-AC47-8AED-43E204B3D6BA}">
-  <dimension ref="A1:C23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
-  <cols>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>